<commit_message>
Latest changes in among other things energy consumption method (including Karpov velocity correction)
</commit_message>
<xml_diff>
--- a/notebooks/Sum_Zuid_Beveland.xlsx
+++ b/notebooks/Sum_Zuid_Beveland.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -655,6 +655,535 @@
         <v>1270</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>517758.6681979147</v>
+      </c>
+      <c r="D10" t="n">
+        <v>7332.199167817354</v>
+      </c>
+      <c r="E10" t="n">
+        <v>244.4447294782518</v>
+      </c>
+      <c r="F10" t="n">
+        <v>668.44367586591</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>517758.6681979147</v>
+      </c>
+      <c r="D11" t="n">
+        <v>7332.199167817354</v>
+      </c>
+      <c r="E11" t="n">
+        <v>244.4447294782518</v>
+      </c>
+      <c r="F11" t="n">
+        <v>668.44367586591</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>110380.789438057</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1563.148976863473</v>
+      </c>
+      <c r="E12" t="n">
+        <v>52.11308640664471</v>
+      </c>
+      <c r="F12" t="n">
+        <v>142.5052735356513</v>
+      </c>
+      <c r="G12" t="n">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>125680.6940147651</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1779.81738726883</v>
+      </c>
+      <c r="E13" t="n">
+        <v>59.33649233935003</v>
+      </c>
+      <c r="F13" t="n">
+        <v>162.2579596494127</v>
+      </c>
+      <c r="G13" t="n">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>145523.4041453484</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2060.818385676509</v>
+      </c>
+      <c r="E14" t="n">
+        <v>68.70465207778945</v>
+      </c>
+      <c r="F14" t="n">
+        <v>187.8755589550305</v>
+      </c>
+      <c r="G14" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>145606.7113463998</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2061.998134140415</v>
+      </c>
+      <c r="E15" t="n">
+        <v>68.74398315537958</v>
+      </c>
+      <c r="F15" t="n">
+        <v>187.9831113246758</v>
+      </c>
+      <c r="G15" t="n">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>145606.7113463998</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2061.998134140415</v>
+      </c>
+      <c r="E16" t="n">
+        <v>68.74398315537958</v>
+      </c>
+      <c r="F16" t="n">
+        <v>187.9831113246758</v>
+      </c>
+      <c r="G16" t="n">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>145606.7113463998</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2061.998134140415</v>
+      </c>
+      <c r="E17" t="n">
+        <v>68.74398315537958</v>
+      </c>
+      <c r="F17" t="n">
+        <v>187.9831113246758</v>
+      </c>
+      <c r="G17" t="n">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>173399.4401752912</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2455.582704917485</v>
+      </c>
+      <c r="E18" t="n">
+        <v>81.8655135077677</v>
+      </c>
+      <c r="F18" t="n">
+        <v>223.8644494110184</v>
+      </c>
+      <c r="G18" t="n">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>173470.1577400294</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2456.584166216959</v>
+      </c>
+      <c r="E19" t="n">
+        <v>81.89890075363716</v>
+      </c>
+      <c r="F19" t="n">
+        <v>223.9557481411622</v>
+      </c>
+      <c r="G19" t="n">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>173470.1577400294</v>
+      </c>
+      <c r="D20" t="n">
+        <v>2456.584166216959</v>
+      </c>
+      <c r="E20" t="n">
+        <v>81.89890075363716</v>
+      </c>
+      <c r="F20" t="n">
+        <v>223.9557481411622</v>
+      </c>
+      <c r="G20" t="n">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>223214.9683322945</v>
+      </c>
+      <c r="D21" t="n">
+        <v>3161.041437988354</v>
+      </c>
+      <c r="E21" t="n">
+        <v>105.3844694467967</v>
+      </c>
+      <c r="F21" t="n">
+        <v>288.1779545278223</v>
+      </c>
+      <c r="G21" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>521779.0801168113</v>
+      </c>
+      <c r="D22" t="n">
+        <v>7389.133918962274</v>
+      </c>
+      <c r="E22" t="n">
+        <v>246.3428502907218</v>
+      </c>
+      <c r="F22" t="n">
+        <v>673.6341614852198</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>529765.3737652395</v>
+      </c>
+      <c r="D23" t="n">
+        <v>7502.231196202831</v>
+      </c>
+      <c r="E23" t="n">
+        <v>250.113347068956</v>
+      </c>
+      <c r="F23" t="n">
+        <v>683.9447324342261</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>550859.0209042045</v>
+      </c>
+      <c r="D24" t="n">
+        <v>7800.947241913791</v>
+      </c>
+      <c r="E24" t="n">
+        <v>260.0721004133788</v>
+      </c>
+      <c r="F24" t="n">
+        <v>711.1773330589144</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>550859.0209042045</v>
+      </c>
+      <c r="D25" t="n">
+        <v>7800.947241913791</v>
+      </c>
+      <c r="E25" t="n">
+        <v>260.0721004133788</v>
+      </c>
+      <c r="F25" t="n">
+        <v>711.1773330589144</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>442612.5120857912</v>
+      </c>
+      <c r="D26" t="n">
+        <v>6268.022714272991</v>
+      </c>
+      <c r="E26" t="n">
+        <v>208.9666526625076</v>
+      </c>
+      <c r="F26" t="n">
+        <v>571.427486849563</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>64059.51804790787</v>
+      </c>
+      <c r="D27" t="n">
+        <v>907.1738896439488</v>
+      </c>
+      <c r="E27" t="n">
+        <v>30.24384239552926</v>
+      </c>
+      <c r="F27" t="n">
+        <v>82.70297022190482</v>
+      </c>
+      <c r="G27" t="n">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>64059.51804790788</v>
+      </c>
+      <c r="D28" t="n">
+        <v>907.1738896439488</v>
+      </c>
+      <c r="E28" t="n">
+        <v>30.24384239552926</v>
+      </c>
+      <c r="F28" t="n">
+        <v>82.70297022190483</v>
+      </c>
+      <c r="G28" t="n">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>237529.6757879372</v>
+      </c>
+      <c r="D29" t="n">
+        <v>3363.758055860908</v>
+      </c>
+      <c r="E29" t="n">
+        <v>112.1427431491664</v>
+      </c>
+      <c r="F29" t="n">
+        <v>306.6587183630671</v>
+      </c>
+      <c r="G29" t="n">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>410999.8335279666</v>
+      </c>
+      <c r="D30" t="n">
+        <v>5820.342222077867</v>
+      </c>
+      <c r="E30" t="n">
+        <v>194.0416439028035</v>
+      </c>
+      <c r="F30" t="n">
+        <v>530.6144665042294</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>172522.4580829261</v>
+      </c>
+      <c r="D31" t="n">
+        <v>2451.859218415024</v>
+      </c>
+      <c r="E31" t="n">
+        <v>81.79114449542097</v>
+      </c>
+      <c r="F31" t="n">
+        <v>222.6579828375058</v>
+      </c>
+      <c r="G31" t="n">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>172522.4580829261</v>
+      </c>
+      <c r="D32" t="n">
+        <v>2451.859218415024</v>
+      </c>
+      <c r="E32" t="n">
+        <v>81.79114449542097</v>
+      </c>
+      <c r="F32" t="n">
+        <v>222.6579828375058</v>
+      </c>
+      <c r="G32" t="n">
+        <v>530</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Latest changes to lock implementation: only implemented Volkerak locks for now. This lock is working now. (changes: changed to graph to a directed graph with two way traffic, because otherwise Dijkstra couldn't read the path; + changed the calling of node names and edges, which worked different for the information loaded from vaarweginformatie.nl)
</commit_message>
<xml_diff>
--- a/notebooks/Sum_Zuid_Beveland.xlsx
+++ b/notebooks/Sum_Zuid_Beveland.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1368,6 +1368,75 @@
         <v>770</v>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B41" t="n">
+        <v>26.42625</v>
+      </c>
+      <c r="C41" t="n">
+        <v>47441.23047591045</v>
+      </c>
+      <c r="D41" t="n">
+        <v>683.8685461702923</v>
+      </c>
+      <c r="E41" t="n">
+        <v>22.86803759909755</v>
+      </c>
+      <c r="F41" t="n">
+        <v>61.14545612816353</v>
+      </c>
+      <c r="G41" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B42" t="n">
+        <v>26.42625</v>
+      </c>
+      <c r="C42" t="n">
+        <v>47441.23047591045</v>
+      </c>
+      <c r="D42" t="n">
+        <v>683.8685461702923</v>
+      </c>
+      <c r="E42" t="n">
+        <v>22.86803759909755</v>
+      </c>
+      <c r="F42" t="n">
+        <v>61.14545612816353</v>
+      </c>
+      <c r="G42" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B43" t="n">
+        <v>26.42625</v>
+      </c>
+      <c r="C43" t="n">
+        <v>47441.23047591045</v>
+      </c>
+      <c r="D43" t="n">
+        <v>683.8685461702923</v>
+      </c>
+      <c r="E43" t="n">
+        <v>22.86803759909755</v>
+      </c>
+      <c r="F43" t="n">
+        <v>61.14545612816353</v>
+      </c>
+      <c r="G43" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>